<commit_message>
Plan de trabajo con actividades hasta el 17
</commit_message>
<xml_diff>
--- a/Plan de Trabajo.xlsx
+++ b/Plan de Trabajo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\danie\Documents\UPIITA-IPN\Quinto-semestre\Ingenieria Web\Ingenieria-Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABA479B-6C62-4061-B070-6EA3F8620F87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3EB22D8-6390-401B-8013-CD702DF929C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Actividades</t>
   </si>
@@ -73,6 +73,18 @@
   </si>
   <si>
     <t>Revision #5 revision/coodinador</t>
+  </si>
+  <si>
+    <t>Todo el equipo</t>
+  </si>
+  <si>
+    <t>Guillermo Ian Rodriguez Mancera</t>
+  </si>
+  <si>
+    <t>Jorge Angel Cruz Meneses</t>
+  </si>
+  <si>
+    <t>Daniel Gonzalez Jimenez</t>
   </si>
 </sst>
 </file>
@@ -95,18 +107,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -140,12 +146,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFBE68E4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -388,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -400,9 +400,34 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -418,33 +443,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,7 +775,7 @@
   <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,64 +785,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="12"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="31"/>
     </row>
     <row r="2" spans="1:14" ht="113.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="13">
+      <c r="A2" s="28"/>
+      <c r="B2" s="7">
         <v>44146</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="8">
         <v>44147</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="8">
         <v>44148</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="8">
         <v>44149</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="8">
         <v>44150</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="8">
         <v>44151</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="8">
         <v>44152</v>
       </c>
-      <c r="I2" s="14">
+      <c r="I2" s="8">
         <v>44153</v>
       </c>
-      <c r="J2" s="14">
+      <c r="J2" s="8">
         <v>44154</v>
       </c>
-      <c r="K2" s="14">
+      <c r="K2" s="8">
         <v>44155</v>
       </c>
-      <c r="L2" s="14">
+      <c r="L2" s="8">
         <v>44156</v>
       </c>
-      <c r="M2" s="14">
+      <c r="M2" s="8">
         <v>44157</v>
       </c>
-      <c r="N2" s="15">
+      <c r="N2" s="9">
         <v>44158</v>
       </c>
     </row>
@@ -844,8 +850,8 @@
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="19"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="13"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -855,15 +861,15 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="7"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="6"/>
     </row>
     <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -873,15 +879,15 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="16"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="10"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="28"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -891,17 +897,17 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="16"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="10"/>
     </row>
     <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="17"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="31"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -909,16 +915,16 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="16"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="10"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="17"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="28"/>
+      <c r="D7" s="22"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -927,15 +933,15 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="16"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="33"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -945,17 +951,17 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="16"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="10"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="17"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="28"/>
+      <c r="E9" s="22"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -963,15 +969,15 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="16"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="10"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="4"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -981,70 +987,112 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="16"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="10"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="17"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="28"/>
+      <c r="G11" s="22"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="16"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="10"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="17"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="18"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="12"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="16"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="10"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="25"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="19"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B15" s="37"/>
+      <c r="C15" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="34"/>
+      <c r="C16" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="35"/>
+      <c r="C17" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="33"/>
+      <c r="C18" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -1052,7 +1100,11 @@
     <row r="33" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C18:H18"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:N1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Correccion de plan de trabajo
</commit_message>
<xml_diff>
--- a/Plan de Trabajo.xlsx
+++ b/Plan de Trabajo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\danie\Documents\UPIITA-IPN\Quinto-semestre\Ingenieria Web\Ingenieria-Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3EB22D8-6390-401B-8013-CD702DF929C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890BA29D-4293-4089-A605-79DF99D26B1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,7 +91,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +102,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -388,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -425,9 +432,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -443,14 +456,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,8 +465,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF1DB954"/>
       <color rgb="FFBE68E4"/>
-      <color rgb="FF1DB954"/>
       <color rgb="FF00FFFF"/>
     </mruColors>
   </colors>
@@ -775,7 +781,7 @@
   <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,27 +791,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="31"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="35"/>
     </row>
     <row r="2" spans="1:14" ht="113.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28"/>
+      <c r="A2" s="32"/>
       <c r="B2" s="7">
         <v>44146</v>
       </c>
@@ -906,8 +912,8 @@
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -940,8 +946,8 @@
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="26"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="25"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -976,8 +982,8 @@
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -1049,48 +1055,48 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="36" t="s">
+      <c r="B15" s="29"/>
+      <c r="C15" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="34"/>
-      <c r="C16" s="36" t="s">
+      <c r="B16" s="27"/>
+      <c r="C16" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="35"/>
-      <c r="C17" s="36" t="s">
+      <c r="B17" s="28"/>
+      <c r="C17" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="33"/>
-      <c r="C18" s="36" t="s">
+      <c r="B18" s="26"/>
+      <c r="C18" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">

</xml_diff>